<commit_message>
finalized plotting and planning
</commit_message>
<xml_diff>
--- a/data/freezing_plotting.xlsx
+++ b/data/freezing_plotting.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/CatherineChamberlain/Documents/git/freezingexperiment/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catchamberlain/Documents/git/freezingexperiment/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9640" yWindow="460" windowWidth="19720" windowHeight="14300" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="300" yWindow="500" windowWidth="30580" windowHeight="26000" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="RED" sheetId="1" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>VIBCAS_W29</t>
   </si>
   <si>
-    <t>ACEPEN_12</t>
-  </si>
-  <si>
     <t>VIBCAS_G28</t>
   </si>
   <si>
@@ -477,9 +474,6 @@
     <t>SAMRAC_G15</t>
   </si>
   <si>
-    <t>SAMRAC_18</t>
-  </si>
-  <si>
     <t>BETPAP_G01</t>
   </si>
   <si>
@@ -508,6 +502,12 @@
   </si>
   <si>
     <t>YELLOW</t>
+  </si>
+  <si>
+    <t>ACEPEN_W12</t>
+  </si>
+  <si>
+    <t>SAMRAC_G18</t>
   </si>
 </sst>
 </file>
@@ -1293,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView zoomScale="68" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A14" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1304,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -1832,7 +1832,7 @@
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
       <c r="AE15" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AF15" s="27"/>
       <c r="AG15" s="5"/>
@@ -2346,7 +2346,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="15" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
@@ -2392,7 +2392,7 @@
       <c r="M29" s="29"/>
       <c r="N29" s="29"/>
       <c r="O29" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P29" s="29"/>
       <c r="Q29" s="29"/>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="AC30" s="5"/>
       <c r="AD30" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE30" s="18"/>
       <c r="AF30" s="26" t="s">
@@ -2529,7 +2529,7 @@
       <c r="U32" s="5"/>
       <c r="V32" s="5"/>
       <c r="W32" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="X32" s="16"/>
       <c r="Y32" s="5"/>
@@ -2558,7 +2558,7 @@
       <c r="K33" s="36"/>
       <c r="L33" s="37"/>
       <c r="M33" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N33" s="36"/>
       <c r="O33" s="38"/>
@@ -2755,7 +2755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="68" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2766,7 +2766,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -3062,7 +3062,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -3076,7 +3076,7 @@
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="U10" s="11"/>
       <c r="V10" s="11"/>
@@ -3284,7 +3284,7 @@
       <c r="Y15" s="5"/>
       <c r="Z15" s="5"/>
       <c r="AA15" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
@@ -3349,7 +3349,7 @@
       <c r="N17" s="29"/>
       <c r="O17" s="31"/>
       <c r="P17" s="29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
@@ -3431,7 +3431,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -3523,7 +3523,7 @@
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
       <c r="X21" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
@@ -3532,7 +3532,7 @@
       <c r="AC21" s="5"/>
       <c r="AD21" s="5"/>
       <c r="AE21" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AF21" s="27"/>
       <c r="AG21" s="5"/>
@@ -3673,7 +3673,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
@@ -3682,7 +3682,7 @@
       <c r="M25" s="29"/>
       <c r="N25" s="29"/>
       <c r="O25" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P25" s="29"/>
       <c r="Q25" s="29"/>
@@ -3690,7 +3690,7 @@
       <c r="S25" s="29"/>
       <c r="T25" s="30"/>
       <c r="U25" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="V25" s="29"/>
       <c r="W25" s="29"/>
@@ -3702,7 +3702,7 @@
       <c r="AC25" s="29"/>
       <c r="AD25" s="29"/>
       <c r="AE25" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AF25" s="27"/>
       <c r="AG25" s="5"/>
@@ -3846,7 +3846,7 @@
       <c r="I29" s="29"/>
       <c r="J29" s="29"/>
       <c r="K29" s="29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L29" s="30"/>
       <c r="M29" s="29"/>
@@ -3854,7 +3854,7 @@
       <c r="O29" s="31"/>
       <c r="P29" s="29"/>
       <c r="Q29" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R29" s="29"/>
       <c r="S29" s="29"/>
@@ -3862,7 +3862,7 @@
       <c r="U29" s="29"/>
       <c r="V29" s="29"/>
       <c r="W29" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X29" s="30"/>
       <c r="Y29" s="29"/>
@@ -3870,7 +3870,7 @@
       <c r="AA29" s="31"/>
       <c r="AB29" s="29"/>
       <c r="AC29" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AD29" s="29"/>
       <c r="AE29" s="32"/>
@@ -4019,7 +4019,7 @@
       <c r="L33" s="37"/>
       <c r="M33" s="36"/>
       <c r="N33" s="36" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O33" s="38"/>
       <c r="P33" s="36"/>
@@ -4028,7 +4028,7 @@
       <c r="S33" s="36"/>
       <c r="T33" s="37"/>
       <c r="U33" s="36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V33" s="36"/>
       <c r="W33" s="36"/>
@@ -4040,7 +4040,7 @@
       <c r="AC33" s="36"/>
       <c r="AD33" s="36"/>
       <c r="AE33" s="39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AF33" s="27"/>
       <c r="AG33" s="5"/>
@@ -4219,7 +4219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView zoomScale="57" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4230,7 +4230,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -4526,7 +4526,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -4540,7 +4540,7 @@
       <c r="R10" s="11"/>
       <c r="S10" s="11"/>
       <c r="T10" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="U10" s="11"/>
       <c r="V10" s="11"/>
@@ -4553,7 +4553,7 @@
       <c r="AC10" s="11"/>
       <c r="AD10" s="11"/>
       <c r="AE10" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AF10" s="5"/>
       <c r="AG10" s="5"/>
@@ -4715,7 +4715,7 @@
       <c r="AC14" s="21"/>
       <c r="AD14" s="21"/>
       <c r="AE14" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AF14" s="26" t="s">
         <v>18</v>
@@ -4815,7 +4815,7 @@
       <c r="N17" s="29"/>
       <c r="O17" s="31"/>
       <c r="P17" s="29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Q17" s="29"/>
       <c r="R17" s="29"/>
@@ -4827,7 +4827,7 @@
       <c r="X17" s="30"/>
       <c r="Y17" s="29"/>
       <c r="Z17" s="29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AA17" s="31"/>
       <c r="AB17" s="29"/>
@@ -4959,7 +4959,7 @@
       <c r="AC20" s="5"/>
       <c r="AD20" s="5"/>
       <c r="AE20" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AF20" s="27"/>
       <c r="AG20" s="5"/>
@@ -4986,14 +4986,14 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="S21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="T21" s="16"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
       <c r="X21" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
@@ -5018,7 +5018,7 @@
         <v>26</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
@@ -5165,7 +5165,7 @@
       <c r="AB25" s="29"/>
       <c r="AC25" s="29"/>
       <c r="AD25" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AE25" s="32"/>
       <c r="AF25" s="27"/>
@@ -5288,7 +5288,7 @@
       <c r="X28" s="16"/>
       <c r="Y28" s="5"/>
       <c r="Z28" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AA28" s="17"/>
       <c r="AB28" s="5"/>
@@ -5315,7 +5315,7 @@
       <c r="L29" s="30"/>
       <c r="M29" s="29"/>
       <c r="N29" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O29" s="31"/>
       <c r="P29" s="29"/>
@@ -5323,7 +5323,7 @@
       <c r="R29" s="29"/>
       <c r="S29" s="29"/>
       <c r="T29" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="U29" s="29"/>
       <c r="V29" s="29"/>
@@ -5485,7 +5485,7 @@
       <c r="P33" s="36"/>
       <c r="Q33" s="36"/>
       <c r="R33" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="S33" s="36"/>
       <c r="T33" s="37"/>
@@ -5677,7 +5677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="62" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -5688,7 +5688,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -5696,7 +5696,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -5984,13 +5984,13 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
       <c r="K10" s="11"/>
       <c r="L10" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
@@ -5998,14 +5998,14 @@
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
       <c r="R10" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S10" s="11"/>
       <c r="T10" s="12"/>
       <c r="U10" s="11"/>
       <c r="V10" s="11"/>
       <c r="W10" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X10" s="12"/>
       <c r="Y10" s="11"/>
@@ -6013,7 +6013,7 @@
       <c r="AA10" s="13"/>
       <c r="AB10" s="11"/>
       <c r="AC10" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AD10" s="11"/>
       <c r="AE10" s="14"/>
@@ -6199,7 +6199,7 @@
       <c r="L15" s="16"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O15" s="17"/>
       <c r="P15" s="5"/>
@@ -6212,7 +6212,7 @@
       <c r="W15" s="5"/>
       <c r="X15" s="16"/>
       <c r="Y15" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Z15" s="5"/>
       <c r="AA15" s="17"/>
@@ -6220,7 +6220,7 @@
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
       <c r="AE15" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AF15" s="27"/>
       <c r="AG15" s="5"/>
@@ -6248,7 +6248,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U16" s="5"/>
       <c r="V16" s="5"/>
@@ -6275,7 +6275,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I17" s="29"/>
       <c r="J17" s="29"/>
@@ -6441,7 +6441,7 @@
       <c r="H21" s="15"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K21" s="5"/>
       <c r="L21" s="16"/>
@@ -6449,7 +6449,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="17"/>
       <c r="P21" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
@@ -6457,19 +6457,19 @@
       <c r="T21" s="16"/>
       <c r="U21" s="5"/>
       <c r="V21" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="W21" s="5"/>
       <c r="X21" s="16"/>
       <c r="Y21" s="5"/>
       <c r="Z21" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AA21" s="17"/>
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AD21" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AE21" s="18"/>
       <c r="AF21" s="27"/>
@@ -6611,7 +6611,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
@@ -6619,7 +6619,7 @@
       <c r="L25" s="30"/>
       <c r="M25" s="29"/>
       <c r="N25" s="29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O25" s="31"/>
       <c r="P25" s="29"/>
@@ -6628,7 +6628,7 @@
       <c r="S25" s="29"/>
       <c r="T25" s="30"/>
       <c r="U25" s="29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="V25" s="29"/>
       <c r="W25" s="29"/>
@@ -6636,13 +6636,13 @@
       <c r="Y25" s="29"/>
       <c r="Z25" s="29"/>
       <c r="AA25" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB25" s="29"/>
       <c r="AC25" s="29"/>
       <c r="AD25" s="29"/>
       <c r="AE25" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AF25" s="27"/>
       <c r="AG25" s="5"/>
@@ -6749,13 +6749,13 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L28" s="16"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P28" s="5"/>
       <c r="Q28" s="5"/>
@@ -6809,7 +6809,7 @@
       <c r="AB29" s="29"/>
       <c r="AC29" s="29"/>
       <c r="AD29" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AE29" s="32"/>
       <c r="AF29" s="27"/>
@@ -6847,7 +6847,7 @@
         <v>43</v>
       </c>
       <c r="U30" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
@@ -6879,7 +6879,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -6937,7 +6937,7 @@
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
       <c r="AA32" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AB32" s="5"/>
       <c r="AC32" s="5"/>
@@ -7157,8 +7157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="52" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7168,7 +7168,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7176,7 +7176,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:35" ht="36" customHeight="1" x14ac:dyDescent="0.2">
@@ -7464,7 +7464,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="11"/>
@@ -7473,7 +7473,7 @@
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P10" s="11"/>
       <c r="Q10" s="11"/>
@@ -7481,7 +7481,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="12"/>
       <c r="U10" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
@@ -7489,7 +7489,7 @@
       <c r="Y10" s="11"/>
       <c r="Z10" s="11"/>
       <c r="AA10" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AB10" s="11"/>
       <c r="AC10" s="11"/>
@@ -7605,7 +7605,7 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AE13" s="18"/>
       <c r="AF13" s="5"/>
@@ -7749,14 +7749,14 @@
       <c r="H17" s="28"/>
       <c r="I17" s="29"/>
       <c r="J17" s="29" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K17" s="29"/>
       <c r="L17" s="30"/>
       <c r="M17" s="29"/>
       <c r="N17" s="29"/>
       <c r="O17" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="P17" s="29"/>
       <c r="Q17" s="29"/>
@@ -7764,7 +7764,7 @@
       <c r="S17" s="29"/>
       <c r="T17" s="30"/>
       <c r="U17" s="29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V17" s="29"/>
       <c r="W17" s="29"/>
@@ -7772,7 +7772,7 @@
       <c r="Y17" s="29"/>
       <c r="Z17" s="29"/>
       <c r="AA17" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AB17" s="29"/>
       <c r="AC17" s="29"/>
@@ -7885,7 +7885,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="16"/>
       <c r="M20" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="N20" s="5"/>
       <c r="O20" s="17"/>
@@ -7929,7 +7929,7 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S21" s="5"/>
       <c r="T21" s="16"/>
@@ -7937,7 +7937,7 @@
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
       <c r="X21" s="16" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
@@ -7962,7 +7962,7 @@
         <v>26</v>
       </c>
       <c r="H22" s="20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
@@ -8071,7 +8071,7 @@
       <c r="AA24" s="17"/>
       <c r="AB24" s="5"/>
       <c r="AC24" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AD24" s="5"/>
       <c r="AE24" s="18"/>
@@ -8097,7 +8097,7 @@
       <c r="N25" s="29"/>
       <c r="O25" s="31"/>
       <c r="P25" s="29" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q25" s="29"/>
       <c r="R25" s="29"/>
@@ -8106,7 +8106,7 @@
       <c r="U25" s="29"/>
       <c r="V25" s="29"/>
       <c r="W25" s="29" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="X25" s="30"/>
       <c r="Y25" s="29"/>
@@ -8184,7 +8184,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L27" s="16"/>
       <c r="M27" s="5"/>
@@ -8243,7 +8243,7 @@
       <c r="AC28" s="5"/>
       <c r="AD28" s="5"/>
       <c r="AE28" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AF28" s="27"/>
       <c r="AG28" s="5"/>
@@ -8269,7 +8269,7 @@
       <c r="P29" s="29"/>
       <c r="Q29" s="29"/>
       <c r="R29" s="29" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="S29" s="29"/>
       <c r="T29" s="30"/>
@@ -8279,7 +8279,7 @@
       <c r="X29" s="30"/>
       <c r="Y29" s="29"/>
       <c r="Z29" s="29" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA29" s="31"/>
       <c r="AB29" s="29"/>
@@ -8429,7 +8429,7 @@
       <c r="J33" s="36"/>
       <c r="K33" s="36"/>
       <c r="L33" s="37" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="M33" s="36"/>
       <c r="N33" s="36"/>
@@ -8448,7 +8448,7 @@
       <c r="AA33" s="38"/>
       <c r="AB33" s="36"/>
       <c r="AC33" s="36" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="AD33" s="36"/>
       <c r="AE33" s="39"/>

</xml_diff>